<commit_message>
start of lesson 3
</commit_message>
<xml_diff>
--- a/M8 prog Planning.xlsx
+++ b/M8 prog Planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Web/ma/m8prog_opdrachtensite/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35339C77-2936-2E45-B930-671B7BF40CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB13EF0-EC70-1741-B84C-FF4602D4C3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="32980" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34460" yWindow="1720" windowWidth="32980" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="planning - Table 1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>week 1</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Custom post type</t>
+  </si>
+  <si>
+    <t>Wordpress Thema installatie</t>
   </si>
 </sst>
 </file>
@@ -1655,7 +1658,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1988,7 +1991,9 @@
     <row r="12" spans="1:12" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="40"/>
       <c r="B12" s="39"/>
-      <c r="C12" s="25"/>
+      <c r="C12" s="30" t="s">
+        <v>47</v>
+      </c>
       <c r="D12" s="25" t="s">
         <v>27</v>
       </c>

</xml_diff>